<commit_message>
On branch amarchan_zc06_vivado_project_dev  Your branch is up-to-date with 'origin/amarchan_zc06_vivado_project_dev'.
 Changes to be committed:
	modified:   compile.xdc
	renamed:    create_athena.tcl -> create_athena_zc706.tcl
	modified:   implementation_timing_constraints.xdc
	modified:   pinout.xdc
	modified:   system.tcl
	modified:   timing.sdc
	modified:   ../../doc/onsemi/xcelerator_fmc_pin_map.xlsx
</commit_message>
<xml_diff>
--- a/athena/doc/onsemi/xcelerator_fmc_pin_map.xlsx
+++ b/athena/doc/onsemi/xcelerator_fmc_pin_map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="230">
   <si>
     <t>Pin No.</t>
   </si>
@@ -689,6 +689,21 @@
   </si>
   <si>
     <t>BOTTOM</t>
+  </si>
+  <si>
+    <t>G18</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>MON_MUX_OUT_VADJ</t>
+  </si>
+  <si>
+    <t>???Not mapped</t>
+  </si>
+  <si>
+    <t>LA16_P</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1238,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1247,6 +1262,7 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1582,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD79"/>
+  <dimension ref="A1:AD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1597,7 +1613,7 @@
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:30" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1639,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:30">
       <c r="A2" s="3" t="s">
         <v>82</v>
       </c>
@@ -1649,7 +1665,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:30">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1675,61 +1691,61 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D4" s="5">
+    <row r="4" spans="1:30">
+      <c r="A4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="G4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>4</v>
@@ -1738,24 +1754,24 @@
         <v>223</v>
       </c>
       <c r="D6" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>4</v>
@@ -1764,1087 +1780,1105 @@
         <v>223</v>
       </c>
       <c r="D7" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
       </c>
       <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" s="8">
+        <v>8</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="10">
+        <v>10</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
         <v>1</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="10">
+        <v>10</v>
+      </c>
+      <c r="E13" s="10">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="10">
+        <v>12</v>
+      </c>
+      <c r="E14" s="10">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="10">
+        <v>12</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="10">
+        <v>14</v>
+      </c>
+      <c r="E16" s="10">
+        <v>2</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" s="10">
+        <v>14</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="13">
+        <v>16</v>
+      </c>
+      <c r="E20" s="13">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" s="13">
+        <v>16</v>
+      </c>
+      <c r="E21" s="13">
+        <v>4</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="15">
+        <v>18</v>
+      </c>
+      <c r="E22" s="15">
+        <v>4</v>
+      </c>
+      <c r="F22" s="15">
+        <v>1</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="15">
+        <v>18</v>
+      </c>
+      <c r="E23" s="15">
+        <v>4</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="15">
+        <v>20</v>
+      </c>
+      <c r="E24" s="15">
+        <v>4</v>
+      </c>
+      <c r="F24" s="15">
+        <v>2</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="15">
+        <v>20</v>
+      </c>
+      <c r="E25" s="15">
+        <v>4</v>
+      </c>
+      <c r="F25" s="15">
+        <v>2</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D26" s="15">
+        <v>22</v>
+      </c>
+      <c r="E26" s="15">
+        <v>4</v>
+      </c>
+      <c r="F26" s="15">
+        <v>3</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D27" s="15">
+        <v>22</v>
+      </c>
+      <c r="E27" s="15">
+        <v>4</v>
+      </c>
+      <c r="F27" s="15">
+        <v>3</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" customFormat="1">
+      <c r="A30" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" s="7">
+        <v>3</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" s="7">
+        <v>3</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="7">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30">
+      <c r="A33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D33" s="7">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="7">
         <v>7</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="18" t="s">
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>3</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30">
+      <c r="A35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D35" s="7">
+        <v>7</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
         <v>3</v>
       </c>
-      <c r="E8" s="7">
+      <c r="G35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30">
+      <c r="A36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" s="9">
+        <v>9</v>
+      </c>
+      <c r="E36" s="9">
+        <v>3</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30">
+      <c r="A37" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D37" s="9">
+        <v>9</v>
+      </c>
+      <c r="E37" s="9">
+        <v>3</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30">
+      <c r="A38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="11">
+        <v>11</v>
+      </c>
+      <c r="E38" s="11">
+        <v>3</v>
+      </c>
+      <c r="F38" s="11">
         <v>1</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G38" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30">
+      <c r="A39" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" s="11">
+        <v>11</v>
+      </c>
+      <c r="E39" s="11">
+        <v>3</v>
+      </c>
+      <c r="F39" s="11">
         <v>1</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="18" t="s">
+      <c r="G39" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D40" s="1">
+        <v>13</v>
+      </c>
+      <c r="E40" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="6">
-        <v>4</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40"/>
+      <c r="AD40"/>
+    </row>
+    <row r="41" spans="1:30">
+      <c r="A41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="11">
+        <v>13</v>
+      </c>
+      <c r="E41" s="11">
+        <v>3</v>
+      </c>
+      <c r="F41" s="11">
+        <v>2</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30">
+      <c r="A42" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="11">
+        <v>15</v>
+      </c>
+      <c r="E42" s="11">
+        <v>3</v>
+      </c>
+      <c r="F42" s="11">
+        <v>3</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30">
+      <c r="A43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="11">
+        <v>15</v>
+      </c>
+      <c r="E43" s="11">
+        <v>3</v>
+      </c>
+      <c r="F43" s="11">
+        <v>3</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30">
+      <c r="A44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="4">
+        <v>3</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30">
+      <c r="A45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="E45" s="23">
+        <v>3</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30">
+      <c r="A46" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="D46" s="14">
+        <v>17</v>
+      </c>
+      <c r="E46" s="14">
+        <v>5</v>
+      </c>
+      <c r="F46" s="14">
         <v>0</v>
       </c>
-      <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="6">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="G46" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30">
+      <c r="A47" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" s="14">
+        <v>17</v>
+      </c>
+      <c r="E47" s="14">
+        <v>5</v>
+      </c>
+      <c r="F47" s="14">
         <v>0</v>
       </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D12" s="7">
-        <v>5</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D13" s="7">
-        <v>5</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" s="6">
-        <v>6</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>3</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D15" s="6">
-        <v>6</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>3</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D16" s="7">
-        <v>7</v>
-      </c>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>3</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30">
-      <c r="A17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D17" s="7">
-        <v>7</v>
-      </c>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7">
-        <v>3</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30">
-      <c r="A18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D18" s="8">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8">
-        <v>2</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30">
-      <c r="A19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D19" s="8">
-        <v>8</v>
-      </c>
-      <c r="E19" s="8">
-        <v>2</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
-      <c r="A20" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D20" s="9">
-        <v>9</v>
-      </c>
-      <c r="E20" s="9">
-        <v>3</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30">
-      <c r="A21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D21" s="9">
-        <v>9</v>
-      </c>
-      <c r="E21" s="9">
-        <v>3</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30">
-      <c r="A22" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D22" s="10">
-        <v>10</v>
-      </c>
-      <c r="E22" s="10">
-        <v>2</v>
-      </c>
-      <c r="F22" s="10">
-        <v>1</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
-      <c r="A23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D23" s="10">
-        <v>10</v>
-      </c>
-      <c r="E23" s="10">
-        <v>2</v>
-      </c>
-      <c r="F23" s="10">
-        <v>1</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30">
-      <c r="A24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D24" s="11">
-        <v>11</v>
-      </c>
-      <c r="E24" s="11">
-        <v>3</v>
-      </c>
-      <c r="F24" s="11">
-        <v>1</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30">
-      <c r="A25" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D25" s="11">
-        <v>11</v>
-      </c>
-      <c r="E25" s="11">
-        <v>3</v>
-      </c>
-      <c r="F25" s="11">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30">
-      <c r="A26" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D26" s="10">
-        <v>12</v>
-      </c>
-      <c r="E26" s="10">
-        <v>2</v>
-      </c>
-      <c r="F26" s="10">
-        <v>2</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30">
-      <c r="A27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D27" s="10">
-        <v>12</v>
-      </c>
-      <c r="E27" s="10">
-        <v>2</v>
-      </c>
-      <c r="F27" s="10">
-        <v>2</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30">
-      <c r="A28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D28" s="1">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1">
-        <v>3</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
-      <c r="P28"/>
-      <c r="Q28"/>
-      <c r="R28"/>
-      <c r="S28"/>
-      <c r="T28"/>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28"/>
-      <c r="X28"/>
-      <c r="Y28"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-      <c r="AB28"/>
-      <c r="AC28"/>
-      <c r="AD28"/>
-    </row>
-    <row r="29" spans="1:30">
-      <c r="A29" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D29" s="11">
-        <v>13</v>
-      </c>
-      <c r="E29" s="11">
-        <v>3</v>
-      </c>
-      <c r="F29" s="11">
-        <v>2</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" customFormat="1">
-      <c r="A30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D30" s="10">
-        <v>14</v>
-      </c>
-      <c r="E30" s="10">
-        <v>2</v>
-      </c>
-      <c r="F30" s="10">
-        <v>3</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:30">
-      <c r="A31" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D31" s="10">
-        <v>14</v>
-      </c>
-      <c r="E31" s="10">
-        <v>2</v>
-      </c>
-      <c r="F31" s="10">
-        <v>3</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30">
-      <c r="A32" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D32" s="11">
-        <v>15</v>
-      </c>
-      <c r="E32" s="11">
-        <v>3</v>
-      </c>
-      <c r="F32" s="11">
-        <v>3</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D33" s="11">
-        <v>15</v>
-      </c>
-      <c r="E33" s="11">
-        <v>3</v>
-      </c>
-      <c r="F33" s="11">
-        <v>3</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D34" s="13">
-        <v>16</v>
-      </c>
-      <c r="E34" s="13">
-        <v>4</v>
-      </c>
-      <c r="F34" s="13">
-        <v>0</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D35" s="13">
-        <v>16</v>
-      </c>
-      <c r="E35" s="13">
-        <v>4</v>
-      </c>
-      <c r="F35" s="13">
-        <v>0</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="D36" s="14">
-        <v>17</v>
-      </c>
-      <c r="E36" s="14">
-        <v>5</v>
-      </c>
-      <c r="F36" s="14">
-        <v>0</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="D37" s="14">
-        <v>17</v>
-      </c>
-      <c r="E37" s="14">
-        <v>5</v>
-      </c>
-      <c r="F37" s="14">
-        <v>0</v>
-      </c>
-      <c r="G37" s="14" t="s">
+      <c r="G47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H47" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D38" s="15">
-        <v>18</v>
-      </c>
-      <c r="E38" s="15">
-        <v>4</v>
-      </c>
-      <c r="F38" s="15">
-        <v>1</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D39" s="15">
-        <v>18</v>
-      </c>
-      <c r="E39" s="15">
-        <v>4</v>
-      </c>
-      <c r="F39" s="15">
-        <v>1</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="16" t="s">
+    <row r="48" spans="1:30">
+      <c r="A48" s="16" t="s">
         <v>123</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D40" s="16">
-        <v>19</v>
-      </c>
-      <c r="E40" s="16">
-        <v>5</v>
-      </c>
-      <c r="F40" s="16">
-        <v>1</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D41" s="16">
-        <v>19</v>
-      </c>
-      <c r="E41" s="16">
-        <v>5</v>
-      </c>
-      <c r="F41" s="16">
-        <v>1</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D42" s="15">
-        <v>20</v>
-      </c>
-      <c r="E42" s="15">
-        <v>4</v>
-      </c>
-      <c r="F42" s="15">
-        <v>2</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D43" s="15">
-        <v>20</v>
-      </c>
-      <c r="E43" s="15">
-        <v>4</v>
-      </c>
-      <c r="F43" s="15">
-        <v>2</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" s="16">
-        <v>21</v>
-      </c>
-      <c r="E44" s="16">
-        <v>5</v>
-      </c>
-      <c r="F44" s="16">
-        <v>2</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" s="16">
-        <v>21</v>
-      </c>
-      <c r="E45" s="16">
-        <v>5</v>
-      </c>
-      <c r="F45" s="16">
-        <v>2</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D46" s="15">
-        <v>22</v>
-      </c>
-      <c r="E46" s="15">
-        <v>4</v>
-      </c>
-      <c r="F46" s="15">
-        <v>3</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="D47" s="15">
-        <v>22</v>
-      </c>
-      <c r="E47" s="15">
-        <v>4</v>
-      </c>
-      <c r="F47" s="15">
-        <v>3</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>4</v>
@@ -2853,24 +2887,24 @@
         <v>224</v>
       </c>
       <c r="D48" s="16">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E48" s="16">
         <v>5</v>
       </c>
       <c r="F48" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>4</v>
@@ -2879,166 +2913,214 @@
         <v>224</v>
       </c>
       <c r="D49" s="16">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E49" s="16">
         <v>5</v>
       </c>
       <c r="F49" s="16">
+        <v>1</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="16">
+        <v>21</v>
+      </c>
+      <c r="E50" s="16">
+        <v>5</v>
+      </c>
+      <c r="F50" s="16">
+        <v>2</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="16">
+        <v>21</v>
+      </c>
+      <c r="E51" s="16">
+        <v>5</v>
+      </c>
+      <c r="F51" s="16">
+        <v>2</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" s="16">
+        <v>23</v>
+      </c>
+      <c r="E52" s="16">
+        <v>5</v>
+      </c>
+      <c r="F52" s="16">
         <v>3</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="G52" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D53" s="16">
+        <v>23</v>
+      </c>
+      <c r="E53" s="16">
+        <v>5</v>
+      </c>
+      <c r="F53" s="16">
+        <v>3</v>
+      </c>
+      <c r="G53" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H53" s="16" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="4" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="4" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="4" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>206</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="4" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>202</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="4" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="4" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>204</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="4" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3274,10 +3356,28 @@
         <v>142</v>
       </c>
     </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:AD79">
+    <sortCondition descending="1" ref="C2:C79"/>
+    <sortCondition ref="E2:E79"/>
     <sortCondition ref="D2:D79"/>
-    <sortCondition ref="G2:G79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>